<commit_message>
added item to todo list (this should be a google doc idk)
</commit_message>
<xml_diff>
--- a/_docs/LD50 task list.xlsx
+++ b/_docs/LD50 task list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lex\Desktop\LD50\LD50\_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B343BE-0E32-4FD3-8257-978D803BDA17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4622A05C-A8D8-4D72-8DE8-6CA4BDF224DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16575" yWindow="3735" windowWidth="27825" windowHeight="17370" xr2:uid="{C126C62B-2136-4544-A8C0-A2BC8919B5DC}"/>
+    <workbookView xWindow="8490" yWindow="1635" windowWidth="27825" windowHeight="17370" xr2:uid="{C126C62B-2136-4544-A8C0-A2BC8919B5DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="68">
   <si>
     <t>Item</t>
   </si>
@@ -236,6 +236,9 @@
   </si>
   <si>
     <t>blocked</t>
+  </si>
+  <si>
+    <t>add bug noise layer to ambience, conditional on proximity to corresponding enclaves</t>
   </si>
 </sst>
 </file>
@@ -641,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04DF0FC1-3919-4ABA-88A7-187EA2AA0198}">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,6 +991,11 @@
       </c>
       <c r="D47" s="3"/>
     </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -995,6 +1003,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D35D80CE318E444F9433E3D20BA6B412" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="184973ce8167093031c80e85d8c428ce">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="6b9e71da-011e-4fca-8c82-41a007b2d43e" xmlns:ns4="71f62a6e-aabe-4272-8fdd-b32a12d066be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b9cc824fd54dde706a29b4a46514124" ns3:_="" ns4:_="">
     <xsd:import namespace="6b9e71da-011e-4fca-8c82-41a007b2d43e"/>
@@ -1217,15 +1234,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1233,6 +1241,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{826D4251-5BAF-438C-8E91-4DE2CC849AAE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCBD8470-7DEB-4B62-9252-0D6FB7E1018F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1247,14 +1263,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{826D4251-5BAF-438C-8E91-4DE2CC849AAE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
made and positioned beetles grouped character position def by village
</commit_message>
<xml_diff>
--- a/_docs/LD50 task list.xlsx
+++ b/_docs/LD50 task list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lex\Desktop\LD50\LD50\_docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lex\Desktop\flickerlight\LD50\LD50\_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4622A05C-A8D8-4D72-8DE8-6CA4BDF224DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC50E04-40FE-4D00-8AE1-098D431E3C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8490" yWindow="1635" windowWidth="27825" windowHeight="17370" xr2:uid="{C126C62B-2136-4544-A8C0-A2BC8919B5DC}"/>
+    <workbookView xWindow="22425" yWindow="2865" windowWidth="27825" windowHeight="17370" xr2:uid="{C126C62B-2136-4544-A8C0-A2BC8919B5DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="70">
   <si>
     <t>Item</t>
   </si>
@@ -239,6 +239,12 @@
   </si>
   <si>
     <t>add bug noise layer to ambience, conditional on proximity to corresponding enclaves</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>AAAA</t>
   </si>
 </sst>
 </file>
@@ -646,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04DF0FC1-3919-4ABA-88A7-187EA2AA0198}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,37 +801,44 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -833,7 +846,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -841,7 +854,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -849,7 +862,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -857,32 +870,32 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -924,10 +937,16 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D39" t="s">
+      <c r="B39" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>54</v>
       </c>
     </row>
@@ -980,16 +999,16 @@
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C47" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D47" s="3"/>
+      <c r="C47" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D47" s="2"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
@@ -1003,15 +1022,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D35D80CE318E444F9433E3D20BA6B412" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="184973ce8167093031c80e85d8c428ce">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="6b9e71da-011e-4fca-8c82-41a007b2d43e" xmlns:ns4="71f62a6e-aabe-4272-8fdd-b32a12d066be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b9cc824fd54dde706a29b4a46514124" ns3:_="" ns4:_="">
     <xsd:import namespace="6b9e71da-011e-4fca-8c82-41a007b2d43e"/>
@@ -1234,6 +1244,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1241,14 +1260,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{826D4251-5BAF-438C-8E91-4DE2CC849AAE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCBD8470-7DEB-4B62-9252-0D6FB7E1018F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1263,6 +1274,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{826D4251-5BAF-438C-8E91-4DE2CC849AAE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>